<commit_message>
+compared data of all models
</commit_message>
<xml_diff>
--- a/data/combinedData.xlsx
+++ b/data/combinedData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Windows\ServiceProfiles\NetworkService\AppData\Local\Packages\oice_16_974fa576_32c1d314_3fa5\AC\Temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakub\PycharmProjects\FantasyPL\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="71" documentId="8_{7C40699A-D3AE-4D2C-B9E1-BCBE6A590D36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46BB5BA6-5AF6-4095-B467-A7D913E75C44}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1593B966-73C7-4ACA-A676-E0EF30805FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="130">
   <si>
     <t>Linear regression</t>
   </si>
@@ -409,6 +409,18 @@
   </si>
   <si>
     <t>tabnet_19_20_gw_0</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Running Total</t>
+  </si>
+  <si>
+    <t>Count</t>
   </si>
 </sst>
 </file>
@@ -894,51 +906,51 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% — akcent 1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% — akcent 2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% — akcent 3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% — akcent 4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% — akcent 5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% — akcent 6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% — akcent 1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% — akcent 2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% — akcent 3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% — akcent 4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% — akcent 5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% — akcent 6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% — akcent 1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% — akcent 2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% — akcent 3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% — akcent 4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% — akcent 5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% — akcent 6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akcent 1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akcent 2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akcent 3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akcent 4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akcent 5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akcent 6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Dane wejściowe" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Dane wyjściowe" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Dobry" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Komórka połączona" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Komórka zaznaczona" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Nagłówek 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Nagłówek 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Nagłówek 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Nagłówek 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Neutralny" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normalny" xfId="0" builtinId="0"/>
-    <cellStyle name="Obliczenia" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Suma" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Tekst objaśnienia" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Tekst ostrzeżenia" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Tytuł" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Uwaga" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Zły" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -954,9 +966,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motyw pakietu Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Pakiet Office">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -994,7 +1006,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Pakiet Office">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1100,7 +1112,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Pakiet Office">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1252,13 +1264,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DQ5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DC1" workbookViewId="0">
-      <selection activeCell="DK7" sqref="DK7"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="AN5" sqref="AN5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:121" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:121" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>106</v>
       </c>
@@ -1278,7 +1290,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:121" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:121" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>5</v>
       </c>
@@ -1352,7 +1364,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:121" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:121" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>107</v>
       </c>
@@ -1702,7 +1714,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="4" spans="1:121" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:121" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>104</v>
       </c>
@@ -1773,13 +1785,13 @@
         <v>34.333760140000003</v>
       </c>
       <c r="X4">
-        <v>1544.818432</v>
+        <v>68.425200000000004</v>
       </c>
       <c r="Y4">
-        <v>336.4286707</v>
+        <v>60.214120000000001</v>
       </c>
       <c r="Z4">
-        <v>1360792740</v>
+        <v>58.423000000000002</v>
       </c>
       <c r="AA4">
         <v>3.4885585236414798</v>
@@ -1791,7 +1803,7 @@
         <v>326.839787</v>
       </c>
       <c r="AD4">
-        <v>2809057.8990000002</v>
+        <v>57.899000000000001</v>
       </c>
       <c r="AE4">
         <v>12.206003490000001</v>
@@ -1806,10 +1818,10 @@
         <v>9.9248385540000008</v>
       </c>
       <c r="AI4">
-        <v>5500.787617</v>
+        <v>55.787616999999997</v>
       </c>
       <c r="AJ4">
-        <v>4054.784353</v>
+        <v>54.784353000000003</v>
       </c>
       <c r="AK4">
         <v>5.9118971938573699</v>
@@ -1821,10 +1833,10 @@
         <v>33.132135130000002</v>
       </c>
       <c r="AN4" s="1">
-        <v>106672000000</v>
+        <v>72.412120000000002</v>
       </c>
       <c r="AO4">
-        <v>1250.1453449999999</v>
+        <v>69.213200000000001</v>
       </c>
       <c r="AP4">
         <v>33.005557138616098</v>
@@ -2067,7 +2079,7 @@
         <v>14.48673902</v>
       </c>
     </row>
-    <row r="5" spans="1:121" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:121" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>105</v>
       </c>
@@ -2186,7 +2198,7 @@
         <v>1944</v>
       </c>
       <c r="AN5">
-        <v>468</v>
+        <v>752</v>
       </c>
       <c r="AO5">
         <v>1066</v>
@@ -2434,5 +2446,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>